<commit_message>
Safety requirements for data updated
</commit_message>
<xml_diff>
--- a/docs/HazardAnalysis/FMEA.xlsx
+++ b/docs/HazardAnalysis/FMEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\Desktop\MECHTRON_4TB6\GitBranch\Capstone_Project\docs\HazardAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CA67A9-57F2-469D-91AA-E5354947EF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DCBC26-7F93-4799-B0F0-B38E933E9D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38E515EC-9FB7-4C21-BAFF-C468AD420BF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Design Component</t>
   </si>
@@ -120,6 +120,18 @@
   <si>
     <t>• Data can't be transferred between hardware and software
 • Lost data</t>
+  </si>
+  <si>
+    <t>All data to be backed up by host software</t>
+  </si>
+  <si>
+    <t>All users required to complete test prompt</t>
+  </si>
+  <si>
+    <t>Only admin users will have access to device manager</t>
+  </si>
+  <si>
+    <t>Safety Requirement</t>
   </si>
 </sst>
 </file>
@@ -230,10 +242,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -561,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD01CFE-8A2C-4743-AAD6-DD0D63AC088F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -575,10 +587,11 @@
     <col min="4" max="4" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -597,53 +610,62 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -655,21 +677,26 @@
       <c r="F4" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="F4:F5"/>

</xml_diff>